<commit_message>
Transaction hw is done
</commit_message>
<xml_diff>
--- a/ADO.NET-Basics/ActionsOnExcel/Points.xlsx
+++ b/ADO.NET-Basics/ActionsOnExcel/Points.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B10" sqref="B10"/>
@@ -501,6 +501,16 @@
         <v>55</v>
       </c>
     </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>Dinko</t>
+        </is>
+      </c>
+      <c r="B12" s="0">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>